<commit_message>
Fitted the vaccine waning
</commit_message>
<xml_diff>
--- a/Model Dependencies/Vaccine efficacy.xlsx
+++ b/Model Dependencies/Vaccine efficacy.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Commuting_TSF_SARS-Cov-2_model_master\Model Dependencies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09EABD8C-6D19-4975-992F-A1AA8C34E734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{187B7B6A-5739-4B2D-8726-1FB9385B1F0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="1" xr2:uid="{37FB83C2-E7A0-4229-A426-40806F42B88C}"/>
+    <workbookView xWindow="-30828" yWindow="-36" windowWidth="30936" windowHeight="16776" xr2:uid="{37FB83C2-E7A0-4229-A426-40806F42B88C}"/>
   </bookViews>
   <sheets>
     <sheet name="10.1056 NEJMoa2118946" sheetId="1" r:id="rId1"/>
     <sheet name="10.1056 NEJMoa2119451" sheetId="2" r:id="rId2"/>
+    <sheet name="BMJ 2022;379 e072141" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="33">
   <si>
     <t>Month</t>
   </si>
@@ -123,22 +124,19 @@
     <t>BNT-162b2</t>
   </si>
   <si>
-    <t>Dose 3</t>
+    <t>Dose</t>
   </si>
   <si>
-    <t>Dose 4</t>
+    <t>Type</t>
   </si>
   <si>
-    <t>Dose 5</t>
+    <t>Effectiveness</t>
   </si>
   <si>
-    <t>Dose 6</t>
+    <t>Effectiveness_min</t>
   </si>
   <si>
-    <t>Dose 7</t>
-  </si>
-  <si>
-    <t>Dose 8</t>
+    <t>Effectiveness_max</t>
   </si>
 </sst>
 </file>
@@ -193,12 +191,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -715,7 +712,553 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'BMJ 2022;379 e072141'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Effectiveness</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'BMJ 2022;379 e072141'!$D$2:$D$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>17</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9B5B-4C62-9444-BB76DFFDF385}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'BMJ 2022;379 e072141'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Effectiveness_min</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'BMJ 2022;379 e072141'!$E$2:$E$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-21</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-48</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-66</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9B5B-4C62-9444-BB76DFFDF385}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'BMJ 2022;379 e072141'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Effectiveness_max</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'BMJ 2022;379 e072141'!$F$2:$F$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>80</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-9B5B-4C62-9444-BB76DFFDF385}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1173206432"/>
+        <c:axId val="1173214336"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1173206432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1173214336"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1173214336"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1173206432"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1271,6 +1814,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1292,6 +2351,47 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0158BAF-33BE-D965-5C8F-91A86B35A7E5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>483576</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>175846</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>1052146</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>17585</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="图表 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{169B619A-8FFB-98E6-C239-E3F0F27AECC9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1611,8 +2711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2DB5C70-D05B-4249-AC4B-963F62CFB1B9}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1965,10 +3065,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{477F4A95-AEC3-42F3-A007-CC92618BB881}">
-  <dimension ref="A1:J44"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1977,14 +3077,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="3"/>
+      <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
       <c r="C2" t="s">
         <v>10</v>
       </c>
@@ -2002,8 +3102,8 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
       <c r="C3" t="s">
         <v>10</v>
       </c>
@@ -2021,8 +3121,8 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
       <c r="C4" t="s">
         <v>11</v>
       </c>
@@ -2040,8 +3140,8 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
       <c r="C5" t="s">
         <v>11</v>
       </c>
@@ -2059,8 +3159,8 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
       <c r="C6" t="s">
         <v>11</v>
       </c>
@@ -2078,8 +3178,8 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
       <c r="C7" t="s">
         <v>11</v>
       </c>
@@ -2097,8 +3197,8 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
       <c r="C8" t="s">
         <v>11</v>
       </c>
@@ -2116,8 +3216,8 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
       <c r="C9" t="s">
         <v>11</v>
       </c>
@@ -2135,8 +3235,8 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
       <c r="C10" t="s">
         <v>11</v>
       </c>
@@ -2154,8 +3254,8 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
       <c r="C11" t="s">
         <v>22</v>
       </c>
@@ -2173,8 +3273,8 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
       <c r="C12" t="s">
         <v>22</v>
       </c>
@@ -2192,8 +3292,8 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
       <c r="C13" t="s">
         <v>22</v>
       </c>
@@ -2211,8 +3311,8 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
       <c r="C14" t="s">
         <v>22</v>
       </c>
@@ -2230,8 +3330,8 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
       <c r="C15" t="s">
         <v>22</v>
       </c>
@@ -2249,8 +3349,8 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
       <c r="C16" t="s">
         <v>25</v>
       </c>
@@ -2268,8 +3368,8 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
       <c r="C17" t="s">
         <v>25</v>
       </c>
@@ -2287,8 +3387,8 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
       <c r="C18" t="s">
         <v>25</v>
       </c>
@@ -2305,23 +3405,11 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-    </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="3"/>
+      <c r="B22" s="2"/>
       <c r="C22" t="s">
         <v>10</v>
       </c>
@@ -2339,8 +3427,8 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
       <c r="C23" t="s">
         <v>10</v>
       </c>
@@ -2358,8 +3446,8 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
       <c r="C24" t="s">
         <v>11</v>
       </c>
@@ -2377,10 +3465,10 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
       <c r="C25" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="D25" t="s">
         <v>15</v>
@@ -2396,10 +3484,10 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
       <c r="C26" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="D26" t="s">
         <v>16</v>
@@ -2415,10 +3503,10 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
       <c r="C27" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="D27" t="s">
         <v>17</v>
@@ -2434,10 +3522,10 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
       <c r="C28" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="D28" t="s">
         <v>18</v>
@@ -2453,10 +3541,10 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
       <c r="C29" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="D29" t="s">
         <v>19</v>
@@ -2472,10 +3560,10 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
       <c r="C30" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="D30" t="s">
         <v>20</v>
@@ -2491,8 +3579,8 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
       <c r="C31" t="s">
         <v>22</v>
       </c>
@@ -2510,8 +3598,8 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="3"/>
-      <c r="B32" s="3"/>
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
       <c r="C32" t="s">
         <v>22</v>
       </c>
@@ -2528,9 +3616,9 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
       <c r="C33" t="s">
         <v>25</v>
       </c>
@@ -2547,28 +3635,28 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
       <c r="C34" t="s">
         <v>25</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D34" t="s">
         <v>23</v>
       </c>
-      <c r="E34" s="2">
+      <c r="E34">
         <v>0.34</v>
       </c>
-      <c r="F34" s="2">
+      <c r="F34">
         <v>0.31</v>
       </c>
-      <c r="G34" s="2">
+      <c r="G34">
         <v>0.36</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
       <c r="C35" t="s">
         <v>25</v>
       </c>
@@ -2585,46 +3673,21 @@
         <v>3.42</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
-      <c r="I37" s="2"/>
-      <c r="J37" s="2"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A38" s="3"/>
-      <c r="B38" s="3"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A39" s="3"/>
-      <c r="B39" s="3"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A40" s="2"/>
-      <c r="B40" s="2"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A42" s="2"/>
-      <c r="B42" s="2"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A43" s="2"/>
-      <c r="B43" s="2"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A44" s="2"/>
-      <c r="B44" s="2"/>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2636,4 +3699,641 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4939171-8CC3-460D-86D0-639FD0066BFB}">
+  <dimension ref="A1:F31"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D20" sqref="A1:F31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.88671875" customWidth="1"/>
+    <col min="3" max="3" width="27" customWidth="1"/>
+    <col min="4" max="4" width="25.88671875" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" customWidth="1"/>
+    <col min="11" max="11" width="14.77734375" customWidth="1"/>
+    <col min="12" max="12" width="16.88671875" customWidth="1"/>
+    <col min="13" max="13" width="16.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>63</v>
+      </c>
+      <c r="E2">
+        <v>46</v>
+      </c>
+      <c r="F2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>55</v>
+      </c>
+      <c r="E3">
+        <v>46</v>
+      </c>
+      <c r="F3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>54</v>
+      </c>
+      <c r="E4">
+        <v>45</v>
+      </c>
+      <c r="F4">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>7</v>
+      </c>
+      <c r="D5">
+        <v>42</v>
+      </c>
+      <c r="E5">
+        <v>34</v>
+      </c>
+      <c r="F5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>9</v>
+      </c>
+      <c r="D6">
+        <v>44</v>
+      </c>
+      <c r="E6">
+        <v>39</v>
+      </c>
+      <c r="F6">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>11</v>
+      </c>
+      <c r="D7">
+        <v>51</v>
+      </c>
+      <c r="E7">
+        <v>46</v>
+      </c>
+      <c r="F7">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>13</v>
+      </c>
+      <c r="D8">
+        <v>32</v>
+      </c>
+      <c r="E8">
+        <v>20</v>
+      </c>
+      <c r="F8">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>15</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>-21</v>
+      </c>
+      <c r="F9">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>17</v>
+      </c>
+      <c r="D10">
+        <v>11</v>
+      </c>
+      <c r="E10">
+        <v>-48</v>
+      </c>
+      <c r="F10">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>88</v>
+      </c>
+      <c r="E11">
+        <v>86</v>
+      </c>
+      <c r="F11">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>85</v>
+      </c>
+      <c r="E12">
+        <v>83</v>
+      </c>
+      <c r="F12">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13">
+        <v>5</v>
+      </c>
+      <c r="D13">
+        <v>66</v>
+      </c>
+      <c r="E13">
+        <v>63</v>
+      </c>
+      <c r="F13">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14">
+        <v>7</v>
+      </c>
+      <c r="D14">
+        <v>33</v>
+      </c>
+      <c r="E14">
+        <v>24</v>
+      </c>
+      <c r="F14">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15">
+        <v>9</v>
+      </c>
+      <c r="D15">
+        <v>32</v>
+      </c>
+      <c r="E15">
+        <v>15</v>
+      </c>
+      <c r="F15">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16">
+        <v>11</v>
+      </c>
+      <c r="D16">
+        <v>17</v>
+      </c>
+      <c r="E16">
+        <v>-66</v>
+      </c>
+      <c r="F16">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>87</v>
+      </c>
+      <c r="E17">
+        <v>75</v>
+      </c>
+      <c r="F17">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <v>74</v>
+      </c>
+      <c r="E18">
+        <v>64</v>
+      </c>
+      <c r="F18">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
+      </c>
+      <c r="D19">
+        <v>64</v>
+      </c>
+      <c r="E19">
+        <v>55</v>
+      </c>
+      <c r="F19">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>7</v>
+      </c>
+      <c r="D20">
+        <v>57</v>
+      </c>
+      <c r="E20">
+        <v>49</v>
+      </c>
+      <c r="F20">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>9</v>
+      </c>
+      <c r="D21">
+        <v>62</v>
+      </c>
+      <c r="E21">
+        <v>57</v>
+      </c>
+      <c r="F21">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>11</v>
+      </c>
+      <c r="D22">
+        <v>61</v>
+      </c>
+      <c r="E22">
+        <v>56</v>
+      </c>
+      <c r="F22">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <v>13</v>
+      </c>
+      <c r="D23">
+        <v>43</v>
+      </c>
+      <c r="E23">
+        <v>30</v>
+      </c>
+      <c r="F23">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <v>15</v>
+      </c>
+      <c r="D24">
+        <v>25</v>
+      </c>
+      <c r="E24">
+        <v>6</v>
+      </c>
+      <c r="F24">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25">
+        <v>17</v>
+      </c>
+      <c r="D25">
+        <v>20</v>
+      </c>
+      <c r="E25">
+        <v>-62</v>
+      </c>
+      <c r="F25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>91</v>
+      </c>
+      <c r="E26">
+        <v>89</v>
+      </c>
+      <c r="F26">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="D27">
+        <v>90</v>
+      </c>
+      <c r="E27">
+        <v>88</v>
+      </c>
+      <c r="F27">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28">
+        <v>5</v>
+      </c>
+      <c r="D28">
+        <v>65</v>
+      </c>
+      <c r="E28">
+        <v>60</v>
+      </c>
+      <c r="F28">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29">
+        <v>7</v>
+      </c>
+      <c r="D29">
+        <v>44</v>
+      </c>
+      <c r="E29">
+        <v>30</v>
+      </c>
+      <c r="F29">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30">
+        <v>9</v>
+      </c>
+      <c r="D30">
+        <v>10</v>
+      </c>
+      <c r="E30">
+        <v>-32</v>
+      </c>
+      <c r="F30">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>